<commit_message>
I updated some of the functions, and built out functionality to add entries to the database, from the spreadsheets that users will submit.  I tested it and my entries have successfully been enterred into my sqlite database.  Next could be building out a GUI, hopefully this will be approved so we can start pumping real data into it, and get further testing and development underway
</commit_message>
<xml_diff>
--- a/test_lineups/ao_scorecard.xlsx
+++ b/test_lineups/ao_scorecard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anthonyperpetua/Desktop/development/fantasy_hvac/test_lineups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF841BBB-2854-E74B-9915-EF77E3359C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DCE1AD-16D7-0445-9FDD-F8F964A51980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20320" xr2:uid="{F8791FE7-8D4D-0143-9C9F-3C69FE54557A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
   <si>
     <t>Week</t>
   </si>
@@ -277,12 +277,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -293,15 +299,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -672,7 +669,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -683,114 +680,144 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="7"/>
     </row>
     <row r="2" spans="1:2" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7"/>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="6"/>
     </row>
     <row r="5" spans="1:2" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="7"/>
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:2" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="7"/>
+      <c r="B6" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:2" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="7"/>
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:2" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="7"/>
+      <c r="B8" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:2" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="7"/>
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="1:2" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="7"/>
+      <c r="B10" s="4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:2" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="7"/>
+      <c r="B11" s="4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:2" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="7"/>
+      <c r="B12" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:2" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="7"/>
+      <c r="B13" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="1:2" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="7"/>
+      <c r="B14" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="15" spans="1:2" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="7"/>
+      <c r="B15" s="4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="16" spans="1:2" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="7"/>
+      <c r="B16" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="17" spans="1:2" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="7"/>
+      <c r="B17" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="18" spans="1:2" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="7"/>
+      <c r="B18" s="4" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>